<commit_message>
[UPDATE] 관리자 > 포인트 하는중 ( cal func )
</commit_message>
<xml_diff>
--- a/라이센스 리셀러 - db.xlsx
+++ b/라이센스 리셀러 - db.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bitnami\wampstack-7.4.29\apache2\htdocs\koi\license_reseller\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA747E41-2875-4F14-80A3-53C8949F94E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31620" windowHeight="14115"/>
+    <workbookView xWindow="7680" yWindow="1275" windowWidth="40635" windowHeight="20670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="105">
   <si>
     <t>기능목록</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -119,10 +120,6 @@
   </si>
   <si>
     <t>od_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스타트업일 경우, 발주서에 금액 표기 X</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -453,7 +450,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -800,11 +797,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="N15:O15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -835,7 +832,7 @@
         <v>17</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>22</v>
@@ -858,13 +855,13 @@
         <v>18</v>
       </c>
       <c r="L2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N2" t="s">
         <v>23</v>
       </c>
       <c r="P2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.3">
@@ -878,16 +875,16 @@
         <v>12</v>
       </c>
       <c r="J3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" t="s">
         <v>47</v>
       </c>
-      <c r="K3" t="s">
-        <v>48</v>
-      </c>
       <c r="L3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="N3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="P3" t="s">
         <v>23</v>
@@ -895,7 +892,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F4" t="s">
         <v>6</v>
@@ -910,19 +907,19 @@
         <v>20</v>
       </c>
       <c r="L4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="N4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="O4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -930,54 +927,51 @@
         <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H5" t="s">
         <v>14</v>
       </c>
       <c r="J5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" t="s">
+        <v>43</v>
+      </c>
+      <c r="M5" t="s">
+        <v>93</v>
+      </c>
+      <c r="N5" t="s">
+        <v>75</v>
+      </c>
+      <c r="O5" t="s">
+        <v>91</v>
+      </c>
+      <c r="P5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" t="s">
         <v>25</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L6" t="s">
         <v>44</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M6" t="s">
         <v>94</v>
       </c>
-      <c r="N5" t="s">
-        <v>76</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="N6" t="s">
+        <v>56</v>
+      </c>
+      <c r="O6" t="s">
         <v>92</v>
       </c>
-      <c r="P5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>75</v>
-      </c>
-      <c r="J6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" t="s">
-        <v>45</v>
-      </c>
-      <c r="M6" t="s">
-        <v>95</v>
-      </c>
-      <c r="N6" t="s">
-        <v>57</v>
-      </c>
-      <c r="O6" t="s">
-        <v>93</v>
-      </c>
       <c r="P6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -985,22 +979,22 @@
         <v>8</v>
       </c>
       <c r="J7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="M7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="P7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -1008,25 +1002,25 @@
         <v>9</v>
       </c>
       <c r="J8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L8" t="s">
+        <v>72</v>
+      </c>
+      <c r="M8" t="s">
         <v>73</v>
       </c>
-      <c r="M8" t="s">
-        <v>74</v>
-      </c>
       <c r="N8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -1034,19 +1028,19 @@
         <v>16</v>
       </c>
       <c r="J9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K9" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="N9" t="s">
+        <v>76</v>
+      </c>
+      <c r="O9" t="s">
         <v>77</v>
-      </c>
-      <c r="O9" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -1054,135 +1048,135 @@
         <v>15</v>
       </c>
       <c r="J10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L11" t="s">
+        <v>99</v>
+      </c>
+      <c r="M11" t="s">
         <v>100</v>
       </c>
-      <c r="M11" t="s">
-        <v>101</v>
-      </c>
       <c r="N11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="N12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="O12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="L15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="L16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="7:14" x14ac:dyDescent="0.3">
       <c r="L17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J21" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="7:14" x14ac:dyDescent="0.3">
       <c r="G22" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="7:14" x14ac:dyDescent="0.3">
       <c r="L23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="M23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>